<commit_message>
Adicionando graficos de estatisticas descritivas e analises de profile
Co-authored-by: Ivan Dobbin <ivandinizdobbin2@gmail.com>
</commit_message>
<xml_diff>
--- a/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
+++ b/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,50 +456,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>m5</t>
+          <t>m6</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>m6</t>
+          <t>repository</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>repository</t>
+          <t>version</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>ncloc</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>ncloc</t>
+          <t>code_quality</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>code_quality</t>
+          <t>testing_status</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>testing_status</t>
+          <t>maintainability</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>maintainability</t>
+          <t>Reliability</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Reliability</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>total</t>
         </is>
@@ -507,10 +502,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1333333333333333</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -519,46 +514,43 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.4</v>
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Archives</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Archives</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
           <t>03-10-2021-15-47</t>
         </is>
       </c>
+      <c r="H2" t="n">
+        <v>239</v>
+      </c>
       <c r="I2" t="n">
-        <v>878</v>
+        <v>0.77</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4400000000000001</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4299999999999999</v>
+        <v>0.385</v>
       </c>
       <c r="L2" t="n">
-        <v>0.22</v>
+        <v>0.5</v>
       </c>
       <c r="M2" t="n">
-        <v>0.215</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.435</v>
+        <v>0.885</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1428571428571428</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -567,46 +559,43 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Archives</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Archives</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
           <t>13-09-2021-15-00</t>
         </is>
       </c>
+      <c r="H3" t="n">
+        <v>109</v>
+      </c>
       <c r="I3" t="n">
-        <v>145</v>
+        <v>0.77</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4478571428571428</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4</v>
+        <v>0.385</v>
       </c>
       <c r="L3" t="n">
-        <v>0.2239285714285714</v>
+        <v>0.4416666666666667</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.4239285714285714</v>
+        <v>0.8266666666666667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1428571428571428</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -615,46 +604,43 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Profile</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Profile</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
           <t>03-10-2021-15-48</t>
         </is>
       </c>
+      <c r="H4" t="n">
+        <v>112</v>
+      </c>
       <c r="I4" t="n">
-        <v>148</v>
+        <v>0.77</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4478571428571428</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4</v>
+        <v>0.385</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2239285714285714</v>
+        <v>0.4416666666666667</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.4239285714285714</v>
+        <v>0.8266666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1428571428571428</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -663,94 +649,88 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Profile</t>
+        </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Profile</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
           <t>13-09-2021-14-00</t>
         </is>
       </c>
+      <c r="H5" t="n">
+        <v>112</v>
+      </c>
       <c r="I5" t="n">
-        <v>148</v>
+        <v>0.77</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4478571428571428</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4</v>
+        <v>0.385</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2239285714285714</v>
+        <v>0.4416666666666667</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.4239285714285714</v>
+        <v>0.8266666666666667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.88</v>
       </c>
       <c r="B6" t="n">
-        <v>0.02222222222222222</v>
+        <v>0.04</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9777777777777777</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.5111111111111111</v>
+        <v>0.92</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Frontend</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
           <t>03-10-2021-15-49</t>
         </is>
       </c>
+      <c r="H6" t="n">
+        <v>1417</v>
+      </c>
       <c r="I6" t="n">
-        <v>2078</v>
+        <v>0.6335999999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>0.638</v>
+        <v>0.944</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5077777777777778</v>
+        <v>0.3168</v>
       </c>
       <c r="L6" t="n">
-        <v>0.319</v>
+        <v>0.472</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2538888888888889</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.5728888888888889</v>
+        <v>0.7887999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -759,86 +739,80 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Frontend</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
           <t>13-09-2021-20-00</t>
         </is>
       </c>
+      <c r="H7" t="n">
+        <v>48</v>
+      </c>
       <c r="I7" t="n">
-        <v>71</v>
+        <v>0.5775</v>
       </c>
       <c r="J7" t="n">
-        <v>0.605</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3833333333333333</v>
+        <v>0.28875</v>
       </c>
       <c r="L7" t="n">
-        <v>0.3025</v>
+        <v>0.325</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1916666666666667</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.4941666666666666</v>
+        <v>0.61375</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.9651162790697675</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01162790697674419</v>
+        <v>0.01923076923076923</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9534883720930233</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.5697674418604651</v>
+        <v>0.9038461538461539</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Frontend</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
           <t>17-10-2021-15-30</t>
         </is>
       </c>
+      <c r="H8" t="n">
+        <v>4874</v>
+      </c>
       <c r="I8" t="n">
-        <v>6662</v>
+        <v>0.6219230769230769</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6369767441860466</v>
+        <v>0.9326923076923077</v>
       </c>
       <c r="K8" t="n">
-        <v>0.5488372093023256</v>
+        <v>0.3109615384615385</v>
       </c>
       <c r="L8" t="n">
-        <v>0.3184883720930233</v>
+        <v>0.4663461538461539</v>
       </c>
       <c r="M8" t="n">
-        <v>0.2744186046511628</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.5929069767441861</v>
+        <v>0.7773076923076923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando novas releases e analisando os graficos
</commit_message>
<xml_diff>
--- a/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
+++ b/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -527,30 +527,30 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>239</v>
+        <v>200</v>
       </c>
       <c r="I2" t="n">
-        <v>0.77</v>
+        <v>0.792</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0.385</v>
+        <v>0.396</v>
       </c>
       <c r="L2" t="n">
         <v>0.5</v>
       </c>
       <c r="M2" t="n">
-        <v>0.885</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -568,26 +568,26 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>13-09-2021-15-00</t>
+          <t>03-11-2021-02-10</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>109</v>
+        <v>428</v>
       </c>
       <c r="I3" t="n">
-        <v>0.77</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8833333333333333</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0.385</v>
+        <v>0.33</v>
       </c>
       <c r="L3" t="n">
-        <v>0.4416666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8266666666666667</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="4">
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -604,35 +604,35 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Profile</t>
+          <t>Archives</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>03-10-2021-15-48</t>
+          <t>13-09-2021-15-00</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I4" t="n">
-        <v>0.77</v>
+        <v>0.792</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8833333333333333</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>0.385</v>
+        <v>0.396</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4416666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8266666666666667</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="5">
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -649,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8333333333333334</v>
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -658,34 +658,34 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>13-09-2021-14-00</t>
+          <t>03-10-2021-15-48</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>112</v>
       </c>
       <c r="I5" t="n">
-        <v>0.77</v>
+        <v>0.792</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8833333333333333</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0.385</v>
+        <v>0.396</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4416666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8266666666666667</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>0.04</v>
+        <v>0.4</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -694,97 +694,97 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Frontend</t>
+          <t>Profile</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>03-10-2021-15-49</t>
+          <t>13-09-2021-14-00</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>1417</v>
+        <v>112</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6335999999999999</v>
+        <v>0.792</v>
       </c>
       <c r="J6" t="n">
-        <v>0.944</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3168</v>
+        <v>0.396</v>
       </c>
       <c r="L6" t="n">
-        <v>0.472</v>
+        <v>0.5</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7887999999999999</v>
+        <v>0.896</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.04545454545454546</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>03-10-2021-15-49</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>1401</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.3225</v>
+      </c>
+      <c r="L7" t="n">
         <v>0.5</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Frontend</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>13-09-2021-20-00</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>48</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.5775</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.6499999999999999</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.28875</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.325</v>
-      </c>
       <c r="M7" t="n">
-        <v>0.61375</v>
+        <v>0.8225</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.9423076923076923</v>
+        <v>0.9591836734693877</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01923076923076923</v>
+        <v>0.02040816326530612</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9230769230769231</v>
+        <v>0.9183673469387755</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9038461538461539</v>
+        <v>0.9387755102040817</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -793,26 +793,116 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
+          <t>03-11-2021-02-08</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>4888</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.626326530612245</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.9571428571428571</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.3131632653061225</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.4785714285714285</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.791734693877551</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>13-09-2021-20-00</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>35</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.8300000000000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.9591836734693877</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.02040816326530612</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9183673469387755</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9591836734693877</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>17-10-2021-15-30</t>
         </is>
       </c>
-      <c r="H8" t="n">
-        <v>4874</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.6219230769230769</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.9326923076923077</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.3109615384615385</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.4663461538461539</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.7773076923076923</v>
+      <c r="H10" t="n">
+        <v>4858</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.626326530612245</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.9714285714285713</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.3131632653061225</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.4857142857142857</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.7988775510204081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ultimas alteracoes notebook (#194)
</commit_message>
<xml_diff>
--- a/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
+++ b/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,42 +461,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>repository</t>
+          <t>Maintainability</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>Reliability</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>ncloc</t>
+          <t>Total_QR</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>code_quality</t>
+          <t>LOC</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>testing_status</t>
+          <t>Repository</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>maintainability</t>
+          <t>Version</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Reliability</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>total</t>
+          <t>Data</t>
         </is>
       </c>
     </row>
@@ -516,33 +511,32 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.896</v>
+      </c>
+      <c r="I2" t="n">
+        <v>200</v>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Archives</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>03-10-2021-15-47</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>200</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.396</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.896</v>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>03-10-2021-15-47</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -561,33 +555,32 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="I3" t="n">
+        <v>428</v>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Archives</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>03-11-2021-02-10</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>428</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.6599999999999999</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.83</v>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>03-11-2021-02-10</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -606,33 +599,32 @@
       <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.896</v>
+      </c>
+      <c r="I4" t="n">
+        <v>109</v>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>Archives</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>13-09-2021-15-00</t>
         </is>
       </c>
-      <c r="H4" t="n">
-        <v>109</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.396</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.896</v>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>13-09-2021-15-00</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -651,33 +643,32 @@
       <c r="E5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.896</v>
+      </c>
+      <c r="I5" t="n">
+        <v>112</v>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>Profile</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>03-10-2021-15-48</t>
         </is>
       </c>
-      <c r="H5" t="n">
-        <v>112</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.396</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.896</v>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>03-10-2021-15-48</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -696,33 +687,32 @@
       <c r="E6" t="n">
         <v>1</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.896</v>
+      </c>
+      <c r="I6" t="n">
+        <v>112</v>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Profile</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>13-09-2021-14-00</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>112</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.792</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.396</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.896</v>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>13-09-2021-14-00</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -741,33 +731,32 @@
       <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>0.3225</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.8225</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1401</v>
+      </c>
+      <c r="J7" t="inlineStr">
         <is>
           <t>Frontend</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>03-10-2021-15-49</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>1401</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.645</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.3225</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.8225</v>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>03-10-2021-15-49</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -786,33 +775,32 @@
       <c r="E8" t="n">
         <v>0.9387755102040817</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>0.3131632653061225</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.4785714285714285</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.791734693877551</v>
+      </c>
+      <c r="I8" t="n">
+        <v>4888</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>Frontend</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>03-11-2021-02-08</t>
         </is>
       </c>
-      <c r="H8" t="n">
-        <v>4888</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.626326530612245</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.9571428571428571</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.3131632653061225</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.4785714285714285</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.791734693877551</v>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>03-11-2021-02-08</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -831,33 +819,32 @@
       <c r="E9" t="n">
         <v>1</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.8300000000000001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>35</v>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>Frontend</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>13-09-2021-20-00</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>35</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.8300000000000001</v>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>13-09-2021-20-00</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -876,33 +863,32 @@
       <c r="E10" t="n">
         <v>0.9591836734693877</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="n">
+        <v>0.3131632653061225</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.4857142857142857</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.7988775510204081</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4858</v>
+      </c>
+      <c r="J10" t="inlineStr">
         <is>
           <t>Frontend</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>17-10-2021-15-30</t>
         </is>
       </c>
-      <c r="H10" t="n">
-        <v>4858</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.626326530612245</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.9714285714285713</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.3131632653061225</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.4857142857142857</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.7988775510204081</v>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>17-10-2021-15-30</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
versao final com ultimas releases
</commit_message>
<xml_diff>
--- a/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
+++ b/analytics-notebooks/data/fga-eps-mds-2021_1-PC-GO1-TO-DATASET-ANALYSIS_DATE.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,10 +585,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -600,16 +600,16 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.396</v>
+        <v>0.3064285714285714</v>
       </c>
       <c r="G4" t="n">
         <v>0.5</v>
       </c>
       <c r="H4" t="n">
-        <v>0.896</v>
+        <v>0.8064285714285715</v>
       </c>
       <c r="I4" t="n">
-        <v>109</v>
+        <v>593</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -618,12 +618,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>13-09-2021-15-00</t>
+          <t>08-11-2021-23-31</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>13-09-2021-15-00</t>
+          <t>08-11-2021-23-31</t>
         </is>
       </c>
     </row>
@@ -653,21 +653,21 @@
         <v>0.896</v>
       </c>
       <c r="I5" t="n">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Profile</t>
+          <t>Archives</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>03-10-2021-15-48</t>
+          <t>13-09-2021-15-00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>03-10-2021-15-48</t>
+          <t>13-09-2021-15-00</t>
         </is>
       </c>
     </row>
@@ -706,21 +706,21 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>13-09-2021-14-00</t>
+          <t>03-10-2021-15-48</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>13-09-2021-14-00</t>
+          <t>03-10-2021-15-48</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.2</v>
       </c>
       <c r="B7" t="n">
-        <v>0.04545454545454546</v>
+        <v>0.4</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -732,83 +732,83 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3225</v>
+        <v>0.264</v>
       </c>
       <c r="G7" t="n">
         <v>0.5</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8225</v>
+        <v>0.764</v>
       </c>
       <c r="I7" t="n">
-        <v>1401</v>
+        <v>155</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Frontend</t>
+          <t>Profile</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>03-10-2021-15-49</t>
+          <t>08-11-2021-23-31</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>03-10-2021-15-49</t>
+          <t>08-11-2021-23-31</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.9591836734693877</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>0.02040816326530612</v>
+        <v>0.4</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9183673469387755</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9387755102040817</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3131632653061225</v>
+        <v>0.396</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4785714285714285</v>
+        <v>0.5</v>
       </c>
       <c r="H8" t="n">
-        <v>0.791734693877551</v>
+        <v>0.896</v>
       </c>
       <c r="I8" t="n">
-        <v>4888</v>
+        <v>112</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Frontend</t>
+          <t>Profile</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>03-11-2021-02-08</t>
+          <t>13-09-2021-14-00</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>03-11-2021-02-08</t>
+          <t>13-09-2021-14-00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.5</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -820,16 +820,16 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.33</v>
+        <v>0.3225</v>
       </c>
       <c r="G9" t="n">
         <v>0.5</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8300000000000001</v>
+        <v>0.8225</v>
       </c>
       <c r="I9" t="n">
-        <v>35</v>
+        <v>1401</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -838,12 +838,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>13-09-2021-20-00</t>
+          <t>03-10-2021-15-49</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>13-09-2021-20-00</t>
+          <t>03-10-2021-15-49</t>
         </is>
       </c>
     </row>
@@ -861,31 +861,163 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9591836734693877</v>
+        <v>0.9387755102040817</v>
       </c>
       <c r="F10" t="n">
         <v>0.3131632653061225</v>
       </c>
       <c r="G10" t="n">
+        <v>0.4785714285714285</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.791734693877551</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4888</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>03-11-2021-02-08</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>03-11-2021-02-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.9607843137254902</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0196078431372549</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.9803921568627451</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.326764705882353</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.4931372549019607</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.8199019607843137</v>
+      </c>
+      <c r="I11" t="n">
+        <v>5638</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>08-11-2021-23-30</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>08-11-2021-23-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.8300000000000001</v>
+      </c>
+      <c r="I12" t="n">
+        <v>35</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>13-09-2021-20-00</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>13-09-2021-20-00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.9591836734693877</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.02040816326530612</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9183673469387755</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.9591836734693877</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3131632653061225</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.4857142857142857</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H13" t="n">
         <v>0.7988775510204081</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I13" t="n">
         <v>4858</v>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Frontend</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>17-10-2021-15-30</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>17-10-2021-15-30</t>
         </is>

</xml_diff>